<commit_message>
Change kill bill reward
</commit_message>
<xml_diff>
--- a/const/kill_bill.xlsx
+++ b/const/kill_bill.xlsx
@@ -385,10 +385,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -747,7 +747,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -765,49 +765,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="8" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="8" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="9" t="s">
         <v>21</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
@@ -817,7 +817,7 @@
       <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
@@ -827,10 +827,10 @@
       <c r="K2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="10"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1">
@@ -1049,10 +1049,10 @@
         <v>9000</v>
       </c>
       <c r="I8" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1">
         <v>1</v>
@@ -1243,10 +1243,10 @@
         <v>32000</v>
       </c>
       <c r="I13" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
@@ -1404,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M17" s="1">
         <v>1</v>
@@ -1436,10 +1436,10 @@
         <v>90000</v>
       </c>
       <c r="I18" s="1">
+        <v>6</v>
+      </c>
+      <c r="J18" s="1">
         <v>3</v>
-      </c>
-      <c r="J18" s="1">
-        <v>4</v>
       </c>
       <c r="K18" s="1">
         <v>1</v>
@@ -1597,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M22" s="1">
         <v>1</v>
@@ -1611,17 +1611,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2040,33 +2040,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
@@ -2076,10 +2076,10 @@
       <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1">

</xml_diff>

<commit_message>
add high level bill
</commit_message>
<xml_diff>
--- a/const/kill_bill.xlsx
+++ b/const/kill_bill.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30140" windowHeight="17380"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="30140" windowHeight="17380"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -329,6 +329,66 @@
   </si>
   <si>
     <t>击败Bill 20</t>
+  </si>
+  <si>
+    <t>Bill's Army 21</t>
+  </si>
+  <si>
+    <t>Bill's Army 22</t>
+  </si>
+  <si>
+    <t>Bill's Army 23</t>
+  </si>
+  <si>
+    <t>Bill's Army 24</t>
+  </si>
+  <si>
+    <t>Bill's Army 25</t>
+  </si>
+  <si>
+    <t>Bill's Army 26</t>
+  </si>
+  <si>
+    <t>Bill's Army 27</t>
+  </si>
+  <si>
+    <t>Bill's Army 28</t>
+  </si>
+  <si>
+    <t>Bill's Army 29</t>
+  </si>
+  <si>
+    <t>Bill's Army 30</t>
+  </si>
+  <si>
+    <t>击败Bill 21</t>
+  </si>
+  <si>
+    <t>击败Bill 22</t>
+  </si>
+  <si>
+    <t>击败Bill 23</t>
+  </si>
+  <si>
+    <t>击败Bill 24</t>
+  </si>
+  <si>
+    <t>击败Bill 25</t>
+  </si>
+  <si>
+    <t>击败Bill 26</t>
+  </si>
+  <si>
+    <t>击败Bill 27</t>
+  </si>
+  <si>
+    <t>击败Bill 28</t>
+  </si>
+  <si>
+    <t>击败Bill 29</t>
+  </si>
+  <si>
+    <t>击败Bill 30</t>
   </si>
 </sst>
 </file>
@@ -404,9 +464,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -447,10 +513,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -460,7 +526,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="24">
     <cellStyle name="标题" xfId="1" builtinId="15"/>
     <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
@@ -470,6 +536,9 @@
     <cellStyle name="超链接" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
@@ -478,6 +547,9 @@
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -808,10 +880,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -829,49 +901,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
@@ -881,7 +953,7 @@
       <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
@@ -891,10 +963,10 @@
       <c r="K2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="10"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1">
@@ -1673,19 +1745,381 @@
         <v>67</v>
       </c>
     </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1">
+        <v>10021</v>
+      </c>
+      <c r="B23" s="1">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="2">
+        <v>15000</v>
+      </c>
+      <c r="H23" s="1">
+        <v>180000</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1">
+        <v>4</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1">
+        <v>10022</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="2">
+        <v>15500</v>
+      </c>
+      <c r="H24" s="1">
+        <v>200000</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1">
+        <v>9</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+      <c r="N24" s="1">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1">
+        <v>10023</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="2">
+        <v>16000</v>
+      </c>
+      <c r="H25" s="1">
+        <v>220000</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>3</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1">
+        <v>3</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="1">
+        <v>10024</v>
+      </c>
+      <c r="B26" s="1">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="2">
+        <v>16500</v>
+      </c>
+      <c r="H26" s="1">
+        <v>240000</v>
+      </c>
+      <c r="I26" s="1">
+        <v>3</v>
+      </c>
+      <c r="J26" s="1">
+        <v>5</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1">
+        <v>46000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="1">
+        <v>10025</v>
+      </c>
+      <c r="B27" s="1">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="2">
+        <v>17000</v>
+      </c>
+      <c r="H27" s="1">
+        <v>260000</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>4</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>3</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="1">
+        <v>10026</v>
+      </c>
+      <c r="B28" s="1">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="2">
+        <v>17500</v>
+      </c>
+      <c r="H28" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1">
+        <v>6</v>
+      </c>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="1">
+        <v>10027</v>
+      </c>
+      <c r="B29" s="1">
+        <v>57</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="2">
+        <v>18000</v>
+      </c>
+      <c r="H29" s="1">
+        <v>300000</v>
+      </c>
+      <c r="I29" s="1">
+        <v>3</v>
+      </c>
+      <c r="J29" s="1">
+        <v>7</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="1">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="1">
+        <v>10028</v>
+      </c>
+      <c r="B30" s="1">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="2">
+        <v>18500</v>
+      </c>
+      <c r="H30" s="1">
+        <v>320000</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>5</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1">
+        <v>3</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="1">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="1">
+        <v>10029</v>
+      </c>
+      <c r="B31" s="1">
+        <v>63</v>
+      </c>
+      <c r="C31" s="1">
+        <v>5</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="2">
+        <v>19000</v>
+      </c>
+      <c r="H31" s="1">
+        <v>340000</v>
+      </c>
+      <c r="I31" s="1">
+        <v>3</v>
+      </c>
+      <c r="J31" s="1">
+        <v>8</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="1">
+        <v>10030</v>
+      </c>
+      <c r="B32" s="1">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="2">
+        <v>19500</v>
+      </c>
+      <c r="H32" s="1">
+        <v>360000</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1">
+        <v>6</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1">
+        <v>3</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+      <c r="N32" s="1">
+        <v>58000</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1700,10 +2134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+      <selection activeCell="B19" sqref="B18:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1877,6 +2311,86 @@
       </c>
       <c r="B21" s="1" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>10021</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>10022</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>10023</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>10024</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>10025</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>10026</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>10027</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>10028</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>10029</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>10030</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1893,10 +2407,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2070,6 +2584,86 @@
       </c>
       <c r="B21" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>10021</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>10022</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>10023</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>10024</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>10025</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>10026</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>10027</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>10028</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>10029</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>10030</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2105,33 +2699,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
@@ -2141,10 +2735,10 @@
       <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1">
@@ -2712,7 +3306,7 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>